<commit_message>
updated obj repo for study files tab; updated icdc profile
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyMGT-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyMGT-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47076270-6061-42F6-A1F9-03769BC26E1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51746B-EB81-4E80-918C-2CA513405E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -75,25 +75,6 @@
 	count(DISTINCT(samp)) as number_of_sample , 
 	count(DISTINCT(c.case_id)) as number_of_cases , 
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment` </t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
@@ -129,6 +110,43 @@
         coalesce(demo.breed,'') AS Breed , 
         coalesce(diag.disease_term,'') AS Diagnosis , 
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)
+  MATCH (demo:demographic) 
+  MATCH (diag:diagnosis)
+ MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+	WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
+OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case)
+OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)&lt;-[:of_sample]-(f:file)
+RETURN 
+	count(DISTINCT(f)) as number_of_files , 
+	count(DISTINCT(samp)) as number_of_sample , 
+	count(DISTINCT(c.case_id)) as number_of_cases , 
+	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
+        coalesce(demo.sex, '') AS Sex ,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment` 
+        coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>StudyFilesTab</t>
   </si>
 </sst>
 </file>
@@ -501,15 +519,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="75.81640625" customWidth="1"/>
     <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -529,15 +547,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -551,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -568,7 +586,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -577,6 +595,23 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
after study files query
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyMGT-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyMGT-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51746B-EB81-4E80-918C-2CA513405E91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC08A8D8-DE87-43CE-9804-A9CEC67FDA9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>WebExcel</t>
   </si>
@@ -126,6 +126,27 @@
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE 
+  s.clinical_study_designation IN ['MGT01'] and
+  demo.breed in ['Australian Cattle Dog','Mixed Breed'] and
+  diag.disease_term in ['Mammary Cancer'] and 
+  diag.primary_disease_site in ['Mammary Gland']
+WITH DISTINCT f, s
+RETURN 
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS `File Format`,
+  coalesce(f.file_size, '') AS `Size`,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
@@ -142,11 +163,8 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment` 
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>StudyFilesTab</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -518,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,12 +565,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -598,12 +616,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>

</xml_diff>